<commit_message>
feat: agregados filtros edad/altura y categorias, columnas descriptivas age/height/weight
</commit_message>
<xml_diff>
--- a/diccionario_metricas_porteros.xlsx
+++ b/diccionario_metricas_porteros.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManuelDuran\AppData\Local\Programs\Python\scouting_porteros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManuelDuran\AppData\Local\Programs\Python\streamlit_scouting_gk\streamlit_scouting_gk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2508EA9-87DA-40CA-8102-0A062F493827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BF2F00-3BD2-4AC3-9420-6E7CB74550BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -626,13 +626,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -941,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -964,10 +963,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>176</v>
       </c>
     </row>
@@ -985,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -1108,13 +1107,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>100</v>
       </c>
       <c r="D10" t="b">
@@ -1125,13 +1124,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>101</v>
       </c>
       <c r="D11" t="b">
@@ -1142,13 +1141,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>102</v>
       </c>
       <c r="D12" t="b">
@@ -1278,7 +1277,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" t="s">
@@ -2350,7 +2349,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B83" t="s">
         <v>89</v>
@@ -2359,15 +2358,15 @@
         <v>160</v>
       </c>
       <c r="D83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B84" t="s">
         <v>90</v>
@@ -2376,15 +2375,15 @@
         <v>161</v>
       </c>
       <c r="D84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B85" t="s">
         <v>91</v>
@@ -2393,10 +2392,10 @@
         <v>162</v>
       </c>
       <c r="D85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustes al input diccionario
</commit_message>
<xml_diff>
--- a/diccionario_metricas_porteros.xlsx
+++ b/diccionario_metricas_porteros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManuelDuran\AppData\Local\Programs\Python\streamlit_scouting_gk\streamlit_scouting_gk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BF2F00-3BD2-4AC3-9420-6E7CB74550BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D0CCDB-18E9-4B47-94C9-35FF60785E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,9 +511,6 @@
     <t>Errores con Gol</t>
   </si>
   <si>
-    <t>Errores con Intento</t>
-  </si>
-  <si>
     <t>Paradas de Baja Intervención</t>
   </si>
   <si>
@@ -541,15 +538,6 @@
     <t>Blocajes Fuera Área Pequeña</t>
   </si>
   <si>
-    <t>Blocajes Fallidos Fuera Área</t>
-  </si>
-  <si>
-    <t>Blocajes Exitosos Fuera Área</t>
-  </si>
-  <si>
-    <t>% Éxito Blocajes Fuera Área</t>
-  </si>
-  <si>
     <t>Invertir</t>
   </si>
   <si>
@@ -557,6 +545,18 @@
   </si>
   <si>
     <t>Centros No Interceptados</t>
+  </si>
+  <si>
+    <t>Errores que terminan en Tiro</t>
+  </si>
+  <si>
+    <t>Blocajes Exitosos Fuera Área Peq.</t>
+  </si>
+  <si>
+    <t>Blocajes Fallidos Fuera Área Peq.</t>
+  </si>
+  <si>
+    <t>% Éxito Blocajes Fuera Área Peq.</t>
   </si>
 </sst>
 </file>
@@ -938,10 +938,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -964,13 +965,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -987,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1038,7 +1039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1055,7 +1056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1072,7 +1073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1089,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1106,7 +1107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1140,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1157,7 +1158,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1165,7 +1166,7 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1174,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1182,7 +1183,7 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1191,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1208,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1242,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1267,7 +1268,7 @@
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -1276,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1284,7 +1285,7 @@
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -1293,7 +1294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1310,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1344,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1361,7 +1362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1378,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1936,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
@@ -1953,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
@@ -1964,7 +1965,7 @@
         <v>66</v>
       </c>
       <c r="C60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -1981,7 +1982,7 @@
         <v>67</v>
       </c>
       <c r="C61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
@@ -1998,7 +1999,7 @@
         <v>68</v>
       </c>
       <c r="C62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -2015,7 +2016,7 @@
         <v>69</v>
       </c>
       <c r="C63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -2032,7 +2033,7 @@
         <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -2049,13 +2050,13 @@
         <v>71</v>
       </c>
       <c r="C65" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
@@ -2066,7 +2067,7 @@
         <v>72</v>
       </c>
       <c r="C66" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -2106,7 +2107,7 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
@@ -2126,7 +2127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -2151,13 +2152,13 @@
         <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D71" t="b">
         <v>1</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.45">
@@ -2174,10 +2175,10 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2194,7 +2195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2211,7 +2212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2228,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2262,7 +2263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2279,7 +2280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -2296,7 +2297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2313,7 +2314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2330,7 +2331,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -2389,7 +2390,7 @@
         <v>91</v>
       </c>
       <c r="C85" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="D85" t="b">
         <v>1</v>
@@ -2399,7 +2400,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E85" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E85" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Construcción"/>
+        <filter val="Juego Aéreo"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización input ponderacion diccionario
</commit_message>
<xml_diff>
--- a/diccionario_metricas_porteros.xlsx
+++ b/diccionario_metricas_porteros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManuelDuran\AppData\Local\Programs\Python\streamlit_scouting_gk\streamlit_scouting_gk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A72918E-61C1-428D-AE7E-6F41830C0440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE61435-EB02-4673-9C80-B5F9DCA9CC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Diccionario" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Diccionario!$A$1:$E$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Diccionario!$A$1:$E$91</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -974,10 +974,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1006,7 +1007,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1023,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1037,10 +1038,10 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1071,10 +1072,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1091,7 +1092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1125,7 +1126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1159,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1176,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1193,7 +1194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1227,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1261,7 +1262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1278,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1292,10 +1293,10 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1329,7 +1330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1346,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1363,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1380,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1397,7 +1398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1414,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1499,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1550,7 +1551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1584,7 +1585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1635,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1683,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
@@ -1737,7 +1738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1788,7 +1789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -1856,7 +1857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.45">
@@ -1958,7 +1959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -1975,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1992,7 +1993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -2009,7 +2010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -2026,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -2043,7 +2044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -2060,7 +2061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -2094,7 +2095,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -2128,7 +2129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -2145,7 +2146,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -2162,7 +2163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -2179,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -2196,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2230,7 +2231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2264,7 +2265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2281,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2298,7 +2299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -2332,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2366,7 +2367,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -2451,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -2468,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>4</v>
       </c>
@@ -2516,7 +2517,7 @@
         <v>0</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.45">
@@ -2537,7 +2538,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E85" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E91" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Construcción"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>